<commit_message>
Partial 15 servo control
</commit_message>
<xml_diff>
--- a/STM32/Leg calibration.xlsx
+++ b/STM32/Leg calibration.xlsx
@@ -287,10 +287,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>121</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -302,13 +302,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>125</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>145</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -323,11 +323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262528424"/>
-        <c:axId val="262523328"/>
+        <c:axId val="96499256"/>
+        <c:axId val="96499648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262528424"/>
+        <c:axId val="96499256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,12 +384,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262523328"/>
+        <c:crossAx val="96499648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262523328"/>
+        <c:axId val="96499648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,7 +446,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262528424"/>
+        <c:crossAx val="96499256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1349,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,13 +1416,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B2">
-        <v>121</v>
-      </c>
-      <c r="C2">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F2">
         <v>-360</v>
@@ -1477,13 +1474,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B4">
-        <v>128</v>
-      </c>
-      <c r="C4">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N16" si="0">N3+1</f>
@@ -1496,11 +1490,11 @@
       </c>
       <c r="B5">
         <f>B4-B2</f>
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:E5" si="1">C4-C2</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
@@ -1520,11 +1514,9 @@
         <v>14</v>
       </c>
       <c r="B6" s="1">
-        <v>-130</v>
-      </c>
-      <c r="C6" s="1">
         <v>-400</v>
       </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="N6">
@@ -1537,10 +1529,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>250</v>
-      </c>
-      <c r="C7">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
@@ -1599,6 +1588,18 @@
       <c r="N16">
         <f t="shared" si="0"/>
         <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <f>118*1.14</f>
+        <v>134.51999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <f>P22*15</f>
+        <v>2017.7999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Single servo code fixed
</commit_message>
<xml_diff>
--- a/STM32/Leg calibration.xlsx
+++ b/STM32/Leg calibration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Desired</t>
   </si>
@@ -73,6 +73,12 @@
   <si>
     <t>c</t>
   </si>
+  <si>
+    <t>Setpoint</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -135,11 +141,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -323,11 +343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96499256"/>
-        <c:axId val="96499648"/>
+        <c:axId val="154220344"/>
+        <c:axId val="155563624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96499256"/>
+        <c:axId val="154220344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,12 +404,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96499648"/>
+        <c:crossAx val="155563624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96499648"/>
+        <c:axId val="155563624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,7 +466,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96499256"/>
+        <c:crossAx val="154220344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1349,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,12 +1385,13 @@
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="6.5703125" customWidth="1"/>
-    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1398,6 +1419,9 @@
         <v>12</v>
       </c>
       <c r="L1" s="3"/>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1413,8 +1437,9 @@
       <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="S1" s="7"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>100</v>
       </c>
@@ -1442,49 +1467,89 @@
         <v>80</v>
       </c>
       <c r="M2">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="N2">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="O2">
-        <v>-140</v>
+        <v>-360</v>
       </c>
       <c r="P2">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="Q2">
         <f>P2+O2*M2/180</f>
-        <v>152.77777777777777</v>
+        <v>140</v>
       </c>
       <c r="R2">
         <f>Q2/107</f>
-        <v>1.4278296988577361</v>
+        <v>1.308411214953271</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>135</v>
+      </c>
+      <c r="M3">
+        <v>110</v>
       </c>
       <c r="N3">
         <f>N2+1</f>
         <v>2</v>
       </c>
+      <c r="O3">
+        <v>-360</v>
+      </c>
+      <c r="P3">
+        <v>305</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q16" si="0">P3+O3*M3/180</f>
+        <v>85</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R17" si="1">Q3/107</f>
+        <v>0.79439252336448596</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>160</v>
       </c>
       <c r="B4">
         <v>167</v>
       </c>
+      <c r="M4">
+        <v>90</v>
+      </c>
       <c r="N4">
-        <f t="shared" ref="N4:N16" si="0">N3+1</f>
+        <f t="shared" ref="N4:N16" si="2">N3+1</f>
         <v>3</v>
       </c>
+      <c r="O4">
+        <v>-363</v>
+      </c>
+      <c r="P4">
+        <v>300</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>118.5</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="1"/>
+        <v>1.1074766355140186</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1493,23 +1558,40 @@
         <v>61</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:E5" si="1">C4-C2</f>
+        <f t="shared" ref="C5:E5" si="3">C4-C2</f>
         <v>0</v>
       </c>
       <c r="D5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>110</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>-365</v>
+      </c>
+      <c r="P5">
+        <v>305</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>81.944444444444457</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0.76583592938733136</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1519,84 +1601,280 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="M6">
+        <v>100</v>
+      </c>
       <c r="N6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>-360</v>
+      </c>
+      <c r="P6">
+        <v>285</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>0.79439252336448596</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B7">
         <v>430</v>
       </c>
+      <c r="M7">
+        <v>110</v>
+      </c>
       <c r="N7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>-400</v>
+      </c>
+      <c r="P7">
+        <v>430</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>185.55555555555554</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>1.7341640706126686</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>110</v>
+      </c>
       <c r="N8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>-400</v>
+      </c>
+      <c r="P8">
+        <v>430</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>185.55555555555554</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>1.7341640706126686</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>110</v>
+      </c>
       <c r="N9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <v>-400</v>
+      </c>
+      <c r="P9">
+        <v>450</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>205.55555555555554</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>1.921079958463136</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>110</v>
+      </c>
       <c r="N10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O10">
+        <v>-400</v>
+      </c>
+      <c r="P10">
+        <v>440</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>195.55555555555554</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>1.8276220145379023</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>110</v>
+      </c>
       <c r="N11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>-400</v>
+      </c>
+      <c r="P11">
+        <v>442</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>197.55555555555554</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>1.846313603322949</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>110</v>
+      </c>
       <c r="N12">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O12">
+        <v>360</v>
+      </c>
+      <c r="P12">
+        <v>-90</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>130</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>1.2149532710280373</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>110</v>
+      </c>
       <c r="N13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O13">
+        <v>545</v>
+      </c>
+      <c r="P13">
+        <v>-112</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>221.05555555555554</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>2.0659397715472481</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>110</v>
+      </c>
       <c r="N14">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O14">
+        <v>490</v>
+      </c>
+      <c r="P14">
+        <v>-105</v>
+      </c>
+      <c r="Q14">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>194.44444444444446</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>1.8172377985462098</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>110</v>
+      </c>
       <c r="N15">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O15">
+        <v>460</v>
+      </c>
+      <c r="P15">
+        <v>-78</v>
+      </c>
+      <c r="Q15">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>203.11111111111109</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>1.8982346832814121</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>110</v>
+      </c>
       <c r="N16">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O16">
+        <v>500</v>
+      </c>
+      <c r="P16">
+        <v>-98</v>
+      </c>
+      <c r="Q16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>207.55555555555554</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>1.9397715472481827</v>
       </c>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>160</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>1.4953271028037383</v>
+      </c>
+    </row>
+    <row r="22" spans="16:18" x14ac:dyDescent="0.25">
       <c r="P22">
         <f>118*1.14</f>
         <v>134.51999999999998</v>
       </c>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="16:18" x14ac:dyDescent="0.25">
       <c r="P23">
         <f>P22*15</f>
         <v>2017.7999999999997</v>
@@ -1606,6 +1884,11 @@
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
+  <conditionalFormatting sqref="S2:S16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"+"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
15 servo code working :-)
</commit_message>
<xml_diff>
--- a/STM32/Leg calibration.xlsx
+++ b/STM32/Leg calibration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Desired</t>
   </si>
@@ -139,10 +139,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -343,11 +343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="154220344"/>
-        <c:axId val="155563624"/>
+        <c:axId val="141596872"/>
+        <c:axId val="141597264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154220344"/>
+        <c:axId val="141596872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,12 +404,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="155563624"/>
+        <c:crossAx val="141597264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="155563624"/>
+        <c:axId val="141597264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +466,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154220344"/>
+        <c:crossAx val="141596872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1371,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,18 +1388,18 @@
     <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.5703125" style="7" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="7"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
@@ -1487,6 +1487,9 @@
         <f>Q2/107</f>
         <v>1.308411214953271</v>
       </c>
+      <c r="S2" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -1513,7 +1516,7 @@
         <f t="shared" ref="R3:R17" si="1">Q3/107</f>
         <v>0.79439252336448596</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1545,7 +1548,7 @@
         <f t="shared" si="1"/>
         <v>1.1074766355140186</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1589,6 +1592,9 @@
       <c r="R5">
         <f t="shared" si="1"/>
         <v>0.76583592938733136</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1622,6 +1628,9 @@
         <f t="shared" si="1"/>
         <v>0.79439252336448596</v>
       </c>
+      <c r="S6" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1651,6 +1660,9 @@
         <f t="shared" si="1"/>
         <v>1.7341640706126686</v>
       </c>
+      <c r="S7" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M8">
@@ -1674,6 +1686,9 @@
         <f t="shared" si="1"/>
         <v>1.7341640706126686</v>
       </c>
+      <c r="S8" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M9">
@@ -1697,6 +1712,9 @@
         <f t="shared" si="1"/>
         <v>1.921079958463136</v>
       </c>
+      <c r="S9" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M10">
@@ -1720,6 +1738,9 @@
         <f t="shared" si="1"/>
         <v>1.8276220145379023</v>
       </c>
+      <c r="S10" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M11">
@@ -1743,6 +1764,9 @@
         <f t="shared" si="1"/>
         <v>1.846313603322949</v>
       </c>
+      <c r="S11" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M12">
@@ -1766,6 +1790,9 @@
         <f t="shared" si="1"/>
         <v>1.2149532710280373</v>
       </c>
+      <c r="S12" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M13">
@@ -1789,6 +1816,9 @@
         <f t="shared" si="1"/>
         <v>2.0659397715472481</v>
       </c>
+      <c r="S13" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M14">
@@ -1812,6 +1842,9 @@
         <f t="shared" si="1"/>
         <v>1.8172377985462098</v>
       </c>
+      <c r="S14" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M15">
@@ -1835,6 +1868,9 @@
         <f t="shared" si="1"/>
         <v>1.8982346832814121</v>
       </c>
+      <c r="S15" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M16">
@@ -1857,6 +1893,9 @@
       <c r="R16">
         <f t="shared" si="1"/>
         <v>1.9397715472481827</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="16:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
something wrong with clock
</commit_message>
<xml_diff>
--- a/STM32/Leg calibration.xlsx
+++ b/STM32/Leg calibration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Desired</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>multiplier</t>
-  </si>
-  <si>
-    <t>ms</t>
   </si>
   <si>
     <t>period</t>
@@ -77,14 +74,26 @@
     <t>Setpoint</t>
   </si>
   <si>
-    <t>+</t>
+    <t>actual ms</t>
+  </si>
+  <si>
+    <t>theory ms</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +105,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -142,6 +159,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -187,6 +214,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>1s Attempt</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -221,16 +273,171 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$S$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$2:$T$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.1588785046729138E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5607476635513993E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2523364485981254E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4164070612668667E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5607476635513993E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5835929387331396E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5835929387331396E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8920041536864067E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2377985462097625E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3686396677050903E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5046728971962704E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1140602284527521</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.2762201453790079E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.1765316718587888E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.10022845275181735</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -261,15 +468,10 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="3.6516185476815399E-2"/>
-                  <c:y val="-0.32916375036453777"/>
-                </c:manualLayout>
-              </c:layout>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -302,38 +504,113 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>Sheet1!$S$2:$S$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>106</c:v>
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>167</c:v>
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>Sheet1!$T$2:$T$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>4.1588785046729138E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>135</c:v>
+                  <c:v>2.5607476635513993E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160</c:v>
+                  <c:v>3.2523364485981254E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4164070612668667E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5607476635513993E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5835929387331396E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5835929387331396E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8920041536864067E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2377985462097625E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3686396677050903E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5046728971962704E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1140602284527521</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.2762201453790079E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.1765316718587888E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.10022845275181735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -343,11 +620,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141596872"/>
-        <c:axId val="141597264"/>
+        <c:axId val="366111056"/>
+        <c:axId val="366109880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141596872"/>
+        <c:axId val="366111056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,12 +681,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141597264"/>
+        <c:crossAx val="366109880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141597264"/>
+        <c:axId val="366109880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +743,403 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141596872"/>
+        <c:crossAx val="366111056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ZA"/>
+              <a:t>2nd</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-ZA" baseline="0"/>
+              <a:t> Attempt</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-ZA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$U$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$V$2:$V$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.1588785046729111E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5607476635514095E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2523364485981459E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4164070612668667E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5607476635514095E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.583592938733136E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.583592938733136E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8920041536863996E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3779854620977758E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6.3136033229489463E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0467289719626773E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.406022845275201E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.2377985462097616E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7653167185878171E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2845275181726521E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="366869736"/>
+        <c:axId val="366877184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="366869736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="366877184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="366877184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="366869736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -555,6 +1228,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1071,24 +1784,540 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1098,6 +2327,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1369,10 +2628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,43 +2645,43 @@
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="6.5703125" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
       <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -1432,19 +2691,30 @@
         <v>3</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="6"/>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>100</v>
       </c>
       <c r="B2">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="F2">
         <v>-360</v>
@@ -1469,7 +2739,7 @@
       <c r="M2">
         <v>80</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="10">
         <f>1</f>
         <v>1</v>
       </c>
@@ -1483,22 +2753,33 @@
         <f>P2+O2*M2/180</f>
         <v>140</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="1">
         <f>Q2/107</f>
         <v>1.308411214953271</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>17</v>
+      <c r="S2" s="6">
+        <v>1.35</v>
+      </c>
+      <c r="T2">
+        <f>(S2-R2)</f>
+        <v>4.1588785046729138E-2</v>
+      </c>
+      <c r="U2">
+        <v>1.32</v>
+      </c>
+      <c r="V2">
+        <f>(U2-R2)</f>
+        <v>1.1588785046729111E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>135</v>
       </c>
       <c r="M3">
         <v>110</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="10">
         <f>N2+1</f>
         <v>2</v>
       </c>
@@ -1516,22 +2797,33 @@
         <f t="shared" ref="R3:R17" si="1">Q3/107</f>
         <v>0.79439252336448596</v>
       </c>
-      <c r="S3" s="6" t="s">
-        <v>17</v>
+      <c r="S3" s="6">
+        <v>0.82</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T16" si="2">(S3-R3)</f>
+        <v>2.5607476635513993E-2</v>
+      </c>
+      <c r="U3">
+        <v>0.81</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V16" si="3">(U3-R3)</f>
+        <v>1.5607476635514095E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B4">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="M4">
         <v>90</v>
       </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N16" si="2">N3+1</f>
+      <c r="N4" s="10">
+        <f t="shared" ref="N4:N16" si="4">N3+1</f>
         <v>3</v>
       </c>
       <c r="O4">
@@ -1548,35 +2840,46 @@
         <f t="shared" si="1"/>
         <v>1.1074766355140186</v>
       </c>
-      <c r="S4" s="6" t="s">
-        <v>17</v>
+      <c r="S4" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="2"/>
+        <v>3.2523364485981254E-2</v>
+      </c>
+      <c r="U4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="3"/>
+        <v>1.2523364485981459E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <f>B4-B2</f>
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:E5" si="3">C4-C2</f>
+        <f t="shared" ref="C5:E5" si="5">C4-C2</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M5">
         <v>110</v>
       </c>
-      <c r="N5">
-        <f t="shared" si="2"/>
+      <c r="N5" s="10">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="O5">
@@ -1593,13 +2896,24 @@
         <f t="shared" si="1"/>
         <v>0.76583592938733136</v>
       </c>
-      <c r="S5" s="6" t="s">
-        <v>17</v>
+      <c r="S5" s="6">
+        <v>0.78</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="2"/>
+        <v>1.4164070612668667E-2</v>
+      </c>
+      <c r="U5">
+        <v>0.78</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="3"/>
+        <v>1.4164070612668667E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>-400</v>
@@ -1610,8 +2924,8 @@
       <c r="M6">
         <v>100</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="2"/>
+      <c r="N6" s="10">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="O6">
@@ -1628,13 +2942,24 @@
         <f t="shared" si="1"/>
         <v>0.79439252336448596</v>
       </c>
-      <c r="S6" s="6" t="s">
-        <v>17</v>
+      <c r="S6" s="6">
+        <v>0.82</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>2.5607476635513993E-2</v>
+      </c>
+      <c r="U6">
+        <v>0.81</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="3"/>
+        <v>1.5607476635514095E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>430</v>
@@ -1642,8 +2967,8 @@
       <c r="M7">
         <v>110</v>
       </c>
-      <c r="N7">
-        <f t="shared" si="2"/>
+      <c r="N7" s="10">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="O7">
@@ -1660,16 +2985,27 @@
         <f t="shared" si="1"/>
         <v>1.7341640706126686</v>
       </c>
-      <c r="S7" s="6" t="s">
-        <v>17</v>
+      <c r="S7" s="6">
+        <v>1.79</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>5.5835929387331396E-2</v>
+      </c>
+      <c r="U7">
+        <v>1.75</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="3"/>
+        <v>1.583592938733136E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M8">
         <v>110</v>
       </c>
-      <c r="N8">
-        <f t="shared" si="2"/>
+      <c r="N8" s="10">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="O8">
@@ -1686,16 +3022,27 @@
         <f t="shared" si="1"/>
         <v>1.7341640706126686</v>
       </c>
-      <c r="S8" s="6" t="s">
-        <v>17</v>
+      <c r="S8" s="6">
+        <v>1.79</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>5.5835929387331396E-2</v>
+      </c>
+      <c r="U8">
+        <v>1.75</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="3"/>
+        <v>1.583592938733136E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M9">
         <v>110</v>
       </c>
-      <c r="N9">
-        <f t="shared" si="2"/>
+      <c r="N9" s="10">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="O9">
@@ -1712,16 +3059,27 @@
         <f t="shared" si="1"/>
         <v>1.921079958463136</v>
       </c>
-      <c r="S9" s="6" t="s">
-        <v>17</v>
+      <c r="S9" s="6">
+        <v>2.02</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>9.8920041536864067E-2</v>
+      </c>
+      <c r="U9">
+        <v>1.94</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="3"/>
+        <v>1.8920041536863996E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M10">
         <v>110</v>
       </c>
-      <c r="N10">
-        <f t="shared" si="2"/>
+      <c r="N10" s="10">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="O10">
@@ -1738,16 +3096,27 @@
         <f t="shared" si="1"/>
         <v>1.8276220145379023</v>
       </c>
-      <c r="S10" s="6" t="s">
-        <v>17</v>
+      <c r="S10" s="6">
+        <v>1.91</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>8.2377985462097625E-2</v>
+      </c>
+      <c r="U10">
+        <v>1.83</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="3"/>
+        <v>2.3779854620977758E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M11">
         <v>110</v>
       </c>
-      <c r="N11">
-        <f t="shared" si="2"/>
+      <c r="N11" s="10">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="O11">
@@ -1764,16 +3133,27 @@
         <f t="shared" si="1"/>
         <v>1.846313603322949</v>
       </c>
-      <c r="S11" s="6" t="s">
-        <v>17</v>
+      <c r="S11" s="6">
+        <v>1.92</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>7.3686396677050903E-2</v>
+      </c>
+      <c r="U11">
+        <v>1.84</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="3"/>
+        <v>-6.3136033229489463E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M12">
         <v>110</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="2"/>
+      <c r="N12" s="10">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="O12">
@@ -1790,16 +3170,27 @@
         <f t="shared" si="1"/>
         <v>1.2149532710280373</v>
       </c>
-      <c r="S12" s="6" t="s">
-        <v>17</v>
+      <c r="S12" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>3.5046728971962704E-2</v>
+      </c>
+      <c r="U12">
+        <v>1.22</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="3"/>
+        <v>5.0467289719626773E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M13">
         <v>110</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="2"/>
+      <c r="N13" s="10">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="O13">
@@ -1816,16 +3207,27 @@
         <f t="shared" si="1"/>
         <v>2.0659397715472481</v>
       </c>
-      <c r="S13" s="6" t="s">
-        <v>17</v>
+      <c r="S13" s="6">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>0.1140602284527521</v>
+      </c>
+      <c r="U13">
+        <v>2.08</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="3"/>
+        <v>1.406022845275201E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M14">
         <v>110</v>
       </c>
-      <c r="N14">
-        <f t="shared" si="2"/>
+      <c r="N14" s="10">
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="O14">
@@ -1842,16 +3244,27 @@
         <f t="shared" si="1"/>
         <v>1.8172377985462098</v>
       </c>
-      <c r="S14" s="6" t="s">
-        <v>17</v>
+      <c r="S14" s="6">
+        <v>1.88</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>6.2762201453790079E-2</v>
+      </c>
+      <c r="U14">
+        <v>1.81</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="3"/>
+        <v>-7.2377985462097616E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M15">
         <v>110</v>
       </c>
-      <c r="N15">
-        <f t="shared" si="2"/>
+      <c r="N15" s="10">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="O15">
@@ -1868,16 +3281,27 @@
         <f t="shared" si="1"/>
         <v>1.8982346832814121</v>
       </c>
-      <c r="S15" s="6" t="s">
-        <v>17</v>
+      <c r="S15" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>8.1765316718587888E-2</v>
+      </c>
+      <c r="U15">
+        <v>1.9</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="3"/>
+        <v>1.7653167185878171E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M16">
         <v>110</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="2"/>
+      <c r="N16" s="10">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="O16">
@@ -1894,29 +3318,19 @@
         <f t="shared" si="1"/>
         <v>1.9397715472481827</v>
       </c>
-      <c r="S16" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="Q17">
-        <v>160</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="1"/>
-        <v>1.4953271028037383</v>
-      </c>
-    </row>
-    <row r="22" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P22">
-        <f>118*1.14</f>
-        <v>134.51999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P23">
-        <f>P22*15</f>
-        <v>2017.7999999999997</v>
+      <c r="S16" s="6">
+        <v>2.04</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>0.10022845275181735</v>
+      </c>
+      <c r="U16">
+        <v>1.94</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="3"/>
+        <v>2.2845275181726521E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Everything up to IK working
</commit_message>
<xml_diff>
--- a/STM32/Leg calibration.xlsx
+++ b/STM32/Leg calibration.xlsx
@@ -161,14 +161,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -620,11 +620,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="366111056"/>
-        <c:axId val="366109880"/>
+        <c:axId val="312464864"/>
+        <c:axId val="312465256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="366111056"/>
+        <c:axId val="312464864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -681,12 +681,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366109880"/>
+        <c:crossAx val="312465256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="366109880"/>
+        <c:axId val="312465256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366111056"/>
+        <c:crossAx val="312464864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1016,11 +1016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="366869736"/>
-        <c:axId val="366877184"/>
+        <c:axId val="313265080"/>
+        <c:axId val="313265472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="366869736"/>
+        <c:axId val="313265080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,12 +1077,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366877184"/>
+        <c:crossAx val="313265472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="366877184"/>
+        <c:axId val="313265472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1139,7 +1139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366869736"/>
+        <c:crossAx val="313265080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2631,7 +2631,7 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,7 +2645,7 @@
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="6.5703125" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5703125" style="6" customWidth="1"/>
   </cols>
@@ -2654,11 +2654,11 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2681,7 +2681,7 @@
       <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -2702,7 +2702,7 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>18</v>
       </c>
       <c r="V1" s="7" t="s">
@@ -2711,10 +2711,16 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>59</v>
+      </c>
+      <c r="C2">
+        <v>65</v>
+      </c>
+      <c r="D2">
+        <v>75</v>
       </c>
       <c r="F2">
         <v>-360</v>
@@ -2739,7 +2745,7 @@
       <c r="M2">
         <v>80</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="9">
         <f>1</f>
         <v>1</v>
       </c>
@@ -2779,7 +2785,7 @@
       <c r="M3">
         <v>110</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <f>N2+1</f>
         <v>2</v>
       </c>
@@ -2794,7 +2800,7 @@
         <v>85</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R17" si="1">Q3/107</f>
+        <f t="shared" ref="R3:R16" si="1">Q3/107</f>
         <v>0.79439252336448596</v>
       </c>
       <c r="S3" s="6">
@@ -2814,15 +2820,21 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="B4">
-        <v>142</v>
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>109</v>
+      </c>
+      <c r="D4">
+        <v>124</v>
       </c>
       <c r="M4">
         <v>90</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <f t="shared" ref="N4:N16" si="4">N3+1</f>
         <v>3</v>
       </c>
@@ -2861,15 +2873,15 @@
       </c>
       <c r="B5">
         <f>B4-B2</f>
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:E5" si="5">C4-C2</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <f t="shared" si="5"/>
@@ -2878,7 +2890,7 @@
       <c r="M5">
         <v>110</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="9">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -2916,15 +2928,17 @@
         <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>-400</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>370</v>
+      </c>
+      <c r="C6" s="1">
+        <v>420</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="M6">
         <v>100</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="9">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -2967,7 +2981,7 @@
       <c r="M7">
         <v>110</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="9">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
@@ -3004,7 +3018,7 @@
       <c r="M8">
         <v>110</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="9">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
@@ -3041,7 +3055,7 @@
       <c r="M9">
         <v>110</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="9">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
@@ -3078,7 +3092,7 @@
       <c r="M10">
         <v>110</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="9">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
@@ -3112,10 +3126,14 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f>120-70</f>
+        <v>50</v>
+      </c>
       <c r="M11">
         <v>110</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="9">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
@@ -3152,7 +3170,7 @@
       <c r="M12">
         <v>110</v>
       </c>
-      <c r="N12" s="10">
+      <c r="N12" s="9">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
@@ -3189,7 +3207,7 @@
       <c r="M13">
         <v>110</v>
       </c>
-      <c r="N13" s="10">
+      <c r="N13" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
@@ -3226,7 +3244,7 @@
       <c r="M14">
         <v>110</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="9">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
@@ -3263,7 +3281,7 @@
       <c r="M15">
         <v>110</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="9">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
@@ -3300,7 +3318,7 @@
       <c r="M16">
         <v>110</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="9">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>

</xml_diff>